<commit_message>
Test Cases updated with AXI_CS_tb results
</commit_message>
<xml_diff>
--- a/Documentation/Test Cases.xlsx
+++ b/Documentation/Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Documents\GitHub\axi2spi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C337EECC-B700-47CF-BF41-0AD3F3C78BAC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70CDF3B-5964-43A5-93C9-E43BF9CE0178}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="308">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t>9a4cd59</t>
+  </si>
+  <si>
+    <t>45e33fa</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1630,6 +1633,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1639,6 +1654,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1647,27 +1692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1951,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26:N37"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N105" sqref="N105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,10 +2042,10 @@
       <c r="G2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="73" t="s">
         <v>305</v>
       </c>
-      <c r="I2" s="80" t="s">
+      <c r="I2" s="75" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2041,8 +2065,8 @@
       <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="81"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
@@ -2054,8 +2078,8 @@
       <c r="E4" s="10"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="81"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="76"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
@@ -2067,8 +2091,8 @@
       <c r="E5" s="11"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="81"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
@@ -2090,10 +2114,10 @@
       <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="74" t="s">
         <v>305</v>
       </c>
-      <c r="I6" s="81" t="s">
+      <c r="I6" s="76" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2113,8 +2137,8 @@
       <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="85"/>
-      <c r="I7" s="81"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="76"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="39"/>
@@ -2126,8 +2150,8 @@
       <c r="E8" s="10"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="81"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="39"/>
@@ -2139,8 +2163,8 @@
       <c r="E9" s="11"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="81"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
@@ -2162,10 +2186,10 @@
       <c r="G10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="85" t="s">
+      <c r="H10" s="74" t="s">
         <v>305</v>
       </c>
-      <c r="I10" s="81" t="s">
+      <c r="I10" s="76" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2185,8 +2209,8 @@
       <c r="G11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="85"/>
-      <c r="I11" s="81"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="76"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
@@ -2198,8 +2222,8 @@
       <c r="E12" s="10"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="81"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="76"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
@@ -2211,8 +2235,8 @@
       <c r="E13" s="11"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="81"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="76"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
@@ -2234,10 +2258,10 @@
       <c r="G14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="85" t="s">
+      <c r="H14" s="74" t="s">
         <v>305</v>
       </c>
-      <c r="I14" s="81" t="s">
+      <c r="I14" s="76" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2257,8 +2281,8 @@
       <c r="G15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="85"/>
-      <c r="I15" s="81"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="76"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
@@ -2270,8 +2294,8 @@
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="81"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="76"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
@@ -2283,8 +2307,8 @@
       <c r="E17" s="11"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="85"/>
-      <c r="I17" s="81"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="76"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
@@ -2306,10 +2330,10 @@
       <c r="G18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="85" t="s">
+      <c r="H18" s="74" t="s">
         <v>305</v>
       </c>
-      <c r="I18" s="81" t="s">
+      <c r="I18" s="76" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2329,8 +2353,8 @@
       <c r="G19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="85"/>
-      <c r="I19" s="81"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="76"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="39"/>
@@ -2342,8 +2366,8 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="81"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="76"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="39"/>
@@ -2355,8 +2379,8 @@
       <c r="E21" s="11"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="81"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="76"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
@@ -2378,10 +2402,10 @@
       <c r="G22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H22" s="82" t="s">
+      <c r="H22" s="87" t="s">
         <v>305</v>
       </c>
-      <c r="I22" s="83" t="s">
+      <c r="I22" s="89" t="s">
         <v>306</v>
       </c>
     </row>
@@ -2401,8 +2425,8 @@
       <c r="G23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="79"/>
-      <c r="I23" s="81"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="76"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
@@ -2414,8 +2438,8 @@
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="81"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="76"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
@@ -2427,11 +2451,11 @@
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="81"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="76"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="77" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="60" t="s">
@@ -2449,12 +2473,18 @@
       <c r="F26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="47"/>
+      <c r="G26" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I26" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="74"/>
+      <c r="A27" s="78"/>
       <c r="B27" s="61"/>
       <c r="C27" s="63"/>
       <c r="D27" s="10" t="s">
@@ -2465,11 +2495,11 @@
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="65"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="84"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="74"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="61"/>
       <c r="C28" s="63"/>
       <c r="D28" s="11" t="s">
@@ -2478,15 +2508,15 @@
       <c r="E28" s="8"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="65"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="89"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="74"/>
+      <c r="A29" s="78"/>
       <c r="B29" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="90" t="s">
         <v>43</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -2498,14 +2528,20 @@
       <c r="F29" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="55"/>
+      <c r="G29" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I29" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="74"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="61"/>
-      <c r="C30" s="76"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="10" t="s">
         <v>44</v>
       </c>
@@ -2514,30 +2550,30 @@
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="65"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="84"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="75"/>
+      <c r="A31" s="79"/>
       <c r="B31" s="67"/>
-      <c r="C31" s="77"/>
+      <c r="C31" s="91"/>
       <c r="D31" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="56"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="84"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="73" t="s">
+      <c r="A32" s="77" t="s">
         <v>46</v>
       </c>
       <c r="B32" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="78" t="s">
+      <c r="C32" s="92" t="s">
         <v>54</v>
       </c>
       <c r="D32" s="14" t="s">
@@ -2549,14 +2585,20 @@
       <c r="F32" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="47"/>
+      <c r="G32" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I32" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="74"/>
+      <c r="A33" s="78"/>
       <c r="B33" s="61"/>
-      <c r="C33" s="76"/>
+      <c r="C33" s="90"/>
       <c r="D33" s="10" t="s">
         <v>29</v>
       </c>
@@ -2565,28 +2607,28 @@
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="65"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="84"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="74"/>
+      <c r="A34" s="78"/>
       <c r="B34" s="61"/>
-      <c r="C34" s="76"/>
+      <c r="C34" s="90"/>
       <c r="D34" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="65"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="89"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="74"/>
+      <c r="A35" s="78"/>
       <c r="B35" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="76" t="s">
+      <c r="C35" s="90" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="9" t="s">
@@ -2598,14 +2640,20 @@
       <c r="F35" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="55"/>
+      <c r="G35" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I35" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="74"/>
+      <c r="A36" s="78"/>
       <c r="B36" s="61"/>
-      <c r="C36" s="76"/>
+      <c r="C36" s="90"/>
       <c r="D36" s="10" t="s">
         <v>58</v>
       </c>
@@ -2614,30 +2662,30 @@
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="65"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="84"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="75"/>
+      <c r="A37" s="79"/>
       <c r="B37" s="67"/>
-      <c r="C37" s="77"/>
+      <c r="C37" s="91"/>
       <c r="D37" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="56"/>
+      <c r="H37" s="86"/>
+      <c r="I37" s="84"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="73" t="s">
+      <c r="A38" s="77" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="78" t="s">
+      <c r="C38" s="92" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="14" t="s">
@@ -2649,14 +2697,20 @@
       <c r="F38" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="47"/>
+      <c r="G38" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I38" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="74"/>
+      <c r="A39" s="78"/>
       <c r="B39" s="61"/>
-      <c r="C39" s="76"/>
+      <c r="C39" s="90"/>
       <c r="D39" s="10" t="s">
         <v>22</v>
       </c>
@@ -2665,28 +2719,28 @@
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="65"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="84"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="74"/>
+      <c r="A40" s="78"/>
       <c r="B40" s="61"/>
-      <c r="C40" s="76"/>
+      <c r="C40" s="90"/>
       <c r="D40" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="65"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="89"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="74"/>
+      <c r="A41" s="78"/>
       <c r="B41" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="90" t="s">
         <v>57</v>
       </c>
       <c r="D41" s="9" t="s">
@@ -2698,14 +2752,20 @@
       <c r="F41" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="55"/>
+      <c r="G41" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H41" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I41" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="74"/>
+      <c r="A42" s="78"/>
       <c r="B42" s="61"/>
-      <c r="C42" s="76"/>
+      <c r="C42" s="90"/>
       <c r="D42" s="10" t="s">
         <v>58</v>
       </c>
@@ -2714,30 +2774,30 @@
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="65"/>
+      <c r="H42" s="81"/>
+      <c r="I42" s="84"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="75"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="67"/>
-      <c r="C43" s="77"/>
+      <c r="C43" s="91"/>
       <c r="D43" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="56"/>
+      <c r="H43" s="86"/>
+      <c r="I43" s="84"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="73" t="s">
+      <c r="A44" s="77" t="s">
         <v>63</v>
       </c>
       <c r="B44" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="78" t="s">
+      <c r="C44" s="92" t="s">
         <v>66</v>
       </c>
       <c r="D44" s="14" t="s">
@@ -2749,14 +2809,20 @@
       <c r="F44" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="47"/>
+      <c r="G44" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H44" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I44" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="74"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="61"/>
-      <c r="C45" s="76"/>
+      <c r="C45" s="90"/>
       <c r="D45" s="10" t="s">
         <v>22</v>
       </c>
@@ -2765,28 +2831,28 @@
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="65"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="84"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="74"/>
+      <c r="A46" s="78"/>
       <c r="B46" s="61"/>
-      <c r="C46" s="76"/>
+      <c r="C46" s="90"/>
       <c r="D46" s="11" t="s">
         <v>69</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="65"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="89"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="74"/>
+      <c r="A47" s="78"/>
       <c r="B47" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="76" t="s">
+      <c r="C47" s="90" t="s">
         <v>67</v>
       </c>
       <c r="D47" s="9" t="s">
@@ -2798,14 +2864,20 @@
       <c r="F47" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="55"/>
+      <c r="G47" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H47" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I47" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="74"/>
+      <c r="A48" s="78"/>
       <c r="B48" s="61"/>
-      <c r="C48" s="76"/>
+      <c r="C48" s="90"/>
       <c r="D48" s="10" t="s">
         <v>68</v>
       </c>
@@ -2814,30 +2886,30 @@
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="65"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="84"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
+      <c r="A49" s="79"/>
       <c r="B49" s="67"/>
-      <c r="C49" s="77"/>
+      <c r="C49" s="91"/>
       <c r="D49" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="16"/>
       <c r="G49" s="16"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="56"/>
+      <c r="H49" s="86"/>
+      <c r="I49" s="84"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="73" t="s">
+      <c r="A50" s="77" t="s">
         <v>73</v>
       </c>
       <c r="B50" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="78" t="s">
+      <c r="C50" s="92" t="s">
         <v>77</v>
       </c>
       <c r="D50" s="14" t="s">
@@ -2849,14 +2921,20 @@
       <c r="F50" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G50" s="14"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="47"/>
+      <c r="G50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H50" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I50" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="74"/>
+      <c r="A51" s="78"/>
       <c r="B51" s="61"/>
-      <c r="C51" s="76"/>
+      <c r="C51" s="90"/>
       <c r="D51" s="10" t="s">
         <v>29</v>
       </c>
@@ -2865,28 +2943,28 @@
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="65"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="84"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="74"/>
+      <c r="A52" s="78"/>
       <c r="B52" s="61"/>
-      <c r="C52" s="76"/>
+      <c r="C52" s="90"/>
       <c r="D52" s="11" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="65"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="89"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="74"/>
+      <c r="A53" s="78"/>
       <c r="B53" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="76" t="s">
+      <c r="C53" s="90" t="s">
         <v>78</v>
       </c>
       <c r="D53" s="9" t="s">
@@ -2898,14 +2976,20 @@
       <c r="F53" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="10"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="55"/>
+      <c r="G53" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I53" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="74"/>
+      <c r="A54" s="78"/>
       <c r="B54" s="61"/>
-      <c r="C54" s="76"/>
+      <c r="C54" s="90"/>
       <c r="D54" s="10" t="s">
         <v>79</v>
       </c>
@@ -2914,30 +2998,30 @@
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="65"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="84"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="75"/>
+      <c r="A55" s="79"/>
       <c r="B55" s="67"/>
-      <c r="C55" s="77"/>
+      <c r="C55" s="91"/>
       <c r="D55" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="16"/>
       <c r="G55" s="16"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="56"/>
+      <c r="H55" s="86"/>
+      <c r="I55" s="84"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="73" t="s">
+      <c r="A56" s="77" t="s">
         <v>85</v>
       </c>
       <c r="B56" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="78" t="s">
+      <c r="C56" s="92" t="s">
         <v>86</v>
       </c>
       <c r="D56" s="14" t="s">
@@ -2949,14 +3033,20 @@
       <c r="F56" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="47"/>
+      <c r="G56" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I56" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="74"/>
+      <c r="A57" s="78"/>
       <c r="B57" s="61"/>
-      <c r="C57" s="76"/>
+      <c r="C57" s="90"/>
       <c r="D57" s="10" t="s">
         <v>22</v>
       </c>
@@ -2965,28 +3055,28 @@
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
-      <c r="H57" s="64"/>
-      <c r="I57" s="65"/>
+      <c r="H57" s="81"/>
+      <c r="I57" s="84"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="74"/>
+      <c r="A58" s="78"/>
       <c r="B58" s="61"/>
-      <c r="C58" s="76"/>
+      <c r="C58" s="90"/>
       <c r="D58" s="11" t="s">
         <v>89</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="65"/>
+      <c r="H58" s="82"/>
+      <c r="I58" s="89"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="74"/>
+      <c r="A59" s="78"/>
       <c r="B59" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="C59" s="76" t="s">
+      <c r="C59" s="90" t="s">
         <v>87</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -2998,14 +3088,20 @@
       <c r="F59" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="55"/>
+      <c r="G59" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H59" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I59" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="74"/>
+      <c r="A60" s="78"/>
       <c r="B60" s="61"/>
-      <c r="C60" s="76"/>
+      <c r="C60" s="90"/>
       <c r="D60" s="10" t="s">
         <v>90</v>
       </c>
@@ -3014,30 +3110,30 @@
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
-      <c r="H60" s="64"/>
-      <c r="I60" s="65"/>
+      <c r="H60" s="81"/>
+      <c r="I60" s="84"/>
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="75"/>
+      <c r="A61" s="79"/>
       <c r="B61" s="67"/>
-      <c r="C61" s="77"/>
+      <c r="C61" s="91"/>
       <c r="D61" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E61" s="17"/>
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
-      <c r="H61" s="54"/>
-      <c r="I61" s="56"/>
+      <c r="H61" s="86"/>
+      <c r="I61" s="84"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="73" t="s">
+      <c r="A62" s="77" t="s">
         <v>93</v>
       </c>
       <c r="B62" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="78" t="s">
+      <c r="C62" s="92" t="s">
         <v>102</v>
       </c>
       <c r="D62" s="14" t="s">
@@ -3049,14 +3145,20 @@
       <c r="F62" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G62" s="14"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="47"/>
+      <c r="G62" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H62" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I62" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="74"/>
+      <c r="A63" s="78"/>
       <c r="B63" s="61"/>
-      <c r="C63" s="76"/>
+      <c r="C63" s="90"/>
       <c r="D63" s="10" t="s">
         <v>29</v>
       </c>
@@ -3065,28 +3167,28 @@
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
-      <c r="H63" s="64"/>
-      <c r="I63" s="65"/>
+      <c r="H63" s="81"/>
+      <c r="I63" s="84"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="74"/>
+      <c r="A64" s="78"/>
       <c r="B64" s="61"/>
-      <c r="C64" s="76"/>
+      <c r="C64" s="90"/>
       <c r="D64" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="65"/>
+      <c r="H64" s="82"/>
+      <c r="I64" s="89"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="74"/>
+      <c r="A65" s="78"/>
       <c r="B65" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="76" t="s">
+      <c r="C65" s="90" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="9" t="s">
@@ -3098,14 +3200,20 @@
       <c r="F65" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G65" s="10"/>
-      <c r="H65" s="53"/>
-      <c r="I65" s="55"/>
+      <c r="G65" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H65" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I65" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="74"/>
+      <c r="A66" s="78"/>
       <c r="B66" s="61"/>
-      <c r="C66" s="76"/>
+      <c r="C66" s="90"/>
       <c r="D66" s="10" t="s">
         <v>104</v>
       </c>
@@ -3114,30 +3222,30 @@
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="65"/>
+      <c r="H66" s="81"/>
+      <c r="I66" s="84"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="75"/>
+      <c r="A67" s="79"/>
       <c r="B67" s="67"/>
-      <c r="C67" s="77"/>
+      <c r="C67" s="91"/>
       <c r="D67" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E67" s="17"/>
       <c r="F67" s="16"/>
       <c r="G67" s="16"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="56"/>
+      <c r="H67" s="86"/>
+      <c r="I67" s="84"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="73" t="s">
+      <c r="A68" s="77" t="s">
         <v>94</v>
       </c>
       <c r="B68" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="78" t="s">
+      <c r="C68" s="92" t="s">
         <v>100</v>
       </c>
       <c r="D68" s="14" t="s">
@@ -3149,14 +3257,20 @@
       <c r="F68" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G68" s="14"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="47"/>
+      <c r="G68" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H68" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I68" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="74"/>
+      <c r="A69" s="78"/>
       <c r="B69" s="61"/>
-      <c r="C69" s="76"/>
+      <c r="C69" s="90"/>
       <c r="D69" s="10" t="s">
         <v>22</v>
       </c>
@@ -3165,28 +3279,28 @@
       </c>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
-      <c r="H69" s="64"/>
-      <c r="I69" s="65"/>
+      <c r="H69" s="81"/>
+      <c r="I69" s="84"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="74"/>
+      <c r="A70" s="78"/>
       <c r="B70" s="61"/>
-      <c r="C70" s="76"/>
+      <c r="C70" s="90"/>
       <c r="D70" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
-      <c r="H70" s="46"/>
-      <c r="I70" s="65"/>
+      <c r="H70" s="82"/>
+      <c r="I70" s="89"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="74"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C71" s="76" t="s">
+      <c r="C71" s="90" t="s">
         <v>99</v>
       </c>
       <c r="D71" s="9" t="s">
@@ -3198,14 +3312,20 @@
       <c r="F71" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G71" s="10"/>
-      <c r="H71" s="53"/>
-      <c r="I71" s="55"/>
+      <c r="G71" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H71" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I71" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="74"/>
+      <c r="A72" s="78"/>
       <c r="B72" s="61"/>
-      <c r="C72" s="76"/>
+      <c r="C72" s="90"/>
       <c r="D72" s="10" t="s">
         <v>104</v>
       </c>
@@ -3214,30 +3334,30 @@
       </c>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
-      <c r="H72" s="64"/>
-      <c r="I72" s="65"/>
+      <c r="H72" s="81"/>
+      <c r="I72" s="84"/>
     </row>
     <row r="73" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="75"/>
+      <c r="A73" s="79"/>
       <c r="B73" s="67"/>
-      <c r="C73" s="77"/>
+      <c r="C73" s="91"/>
       <c r="D73" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E73" s="17"/>
       <c r="F73" s="16"/>
       <c r="G73" s="16"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="56"/>
+      <c r="H73" s="86"/>
+      <c r="I73" s="84"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="73" t="s">
+      <c r="A74" s="77" t="s">
         <v>109</v>
       </c>
       <c r="B74" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="C74" s="78" t="s">
+      <c r="C74" s="92" t="s">
         <v>111</v>
       </c>
       <c r="D74" s="14" t="s">
@@ -3249,14 +3369,20 @@
       <c r="F74" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="G74" s="14"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="47"/>
+      <c r="G74" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H74" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I74" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="74"/>
+      <c r="A75" s="78"/>
       <c r="B75" s="61"/>
-      <c r="C75" s="76"/>
+      <c r="C75" s="90"/>
       <c r="D75" s="10" t="s">
         <v>22</v>
       </c>
@@ -3265,28 +3391,28 @@
       </c>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
-      <c r="H75" s="64"/>
-      <c r="I75" s="65"/>
+      <c r="H75" s="81"/>
+      <c r="I75" s="84"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="74"/>
+      <c r="A76" s="78"/>
       <c r="B76" s="61"/>
-      <c r="C76" s="76"/>
+      <c r="C76" s="90"/>
       <c r="D76" s="11" t="s">
         <v>114</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
-      <c r="H76" s="46"/>
-      <c r="I76" s="65"/>
+      <c r="H76" s="82"/>
+      <c r="I76" s="89"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="74"/>
+      <c r="A77" s="78"/>
       <c r="B77" s="61" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="76" t="s">
+      <c r="C77" s="90" t="s">
         <v>110</v>
       </c>
       <c r="D77" s="9" t="s">
@@ -3298,14 +3424,20 @@
       <c r="F77" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G77" s="10"/>
-      <c r="H77" s="53"/>
-      <c r="I77" s="55"/>
+      <c r="G77" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H77" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I77" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="74"/>
+      <c r="A78" s="78"/>
       <c r="B78" s="61"/>
-      <c r="C78" s="76"/>
+      <c r="C78" s="90"/>
       <c r="D78" s="10" t="s">
         <v>113</v>
       </c>
@@ -3314,30 +3446,30 @@
       </c>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
-      <c r="H78" s="64"/>
-      <c r="I78" s="65"/>
+      <c r="H78" s="81"/>
+      <c r="I78" s="84"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="75"/>
+      <c r="A79" s="79"/>
       <c r="B79" s="67"/>
-      <c r="C79" s="77"/>
+      <c r="C79" s="91"/>
       <c r="D79" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E79" s="17"/>
       <c r="F79" s="16"/>
       <c r="G79" s="16"/>
-      <c r="H79" s="54"/>
-      <c r="I79" s="56"/>
+      <c r="H79" s="86"/>
+      <c r="I79" s="84"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="77" t="s">
         <v>119</v>
       </c>
       <c r="B80" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="C80" s="78" t="s">
+      <c r="C80" s="92" t="s">
         <v>123</v>
       </c>
       <c r="D80" s="14" t="s">
@@ -3349,14 +3481,20 @@
       <c r="F80" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G80" s="14"/>
-      <c r="H80" s="45"/>
-      <c r="I80" s="47"/>
+      <c r="G80" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H80" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I80" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="74"/>
+      <c r="A81" s="78"/>
       <c r="B81" s="61"/>
-      <c r="C81" s="76"/>
+      <c r="C81" s="90"/>
       <c r="D81" s="10" t="s">
         <v>22</v>
       </c>
@@ -3365,28 +3503,28 @@
       </c>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
-      <c r="H81" s="64"/>
-      <c r="I81" s="65"/>
+      <c r="H81" s="81"/>
+      <c r="I81" s="84"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="74"/>
+      <c r="A82" s="78"/>
       <c r="B82" s="61"/>
-      <c r="C82" s="76"/>
+      <c r="C82" s="90"/>
       <c r="D82" s="11" t="s">
         <v>126</v>
       </c>
       <c r="E82" s="8"/>
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="65"/>
+      <c r="H82" s="82"/>
+      <c r="I82" s="89"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="74"/>
+      <c r="A83" s="78"/>
       <c r="B83" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="C83" s="76" t="s">
+      <c r="C83" s="90" t="s">
         <v>122</v>
       </c>
       <c r="D83" s="9" t="s">
@@ -3398,14 +3536,20 @@
       <c r="F83" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="G83" s="10"/>
-      <c r="H83" s="53"/>
-      <c r="I83" s="55"/>
+      <c r="G83" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H83" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I83" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="74"/>
+      <c r="A84" s="78"/>
       <c r="B84" s="61"/>
-      <c r="C84" s="76"/>
+      <c r="C84" s="90"/>
       <c r="D84" s="10" t="s">
         <v>125</v>
       </c>
@@ -3414,30 +3558,30 @@
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
-      <c r="H84" s="64"/>
-      <c r="I84" s="65"/>
+      <c r="H84" s="81"/>
+      <c r="I84" s="84"/>
     </row>
     <row r="85" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="75"/>
+      <c r="A85" s="79"/>
       <c r="B85" s="67"/>
-      <c r="C85" s="77"/>
+      <c r="C85" s="91"/>
       <c r="D85" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E85" s="17"/>
       <c r="F85" s="16"/>
       <c r="G85" s="16"/>
-      <c r="H85" s="54"/>
-      <c r="I85" s="56"/>
+      <c r="H85" s="86"/>
+      <c r="I85" s="84"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="73" t="s">
+      <c r="A86" s="77" t="s">
         <v>129</v>
       </c>
       <c r="B86" s="60" t="s">
         <v>131</v>
       </c>
-      <c r="C86" s="78" t="s">
+      <c r="C86" s="92" t="s">
         <v>138</v>
       </c>
       <c r="D86" s="14" t="s">
@@ -3449,14 +3593,20 @@
       <c r="F86" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G86" s="14"/>
-      <c r="H86" s="45"/>
-      <c r="I86" s="47"/>
+      <c r="G86" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="H86" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I86" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="74"/>
+      <c r="A87" s="78"/>
       <c r="B87" s="61"/>
-      <c r="C87" s="76"/>
+      <c r="C87" s="90"/>
       <c r="D87" s="10" t="s">
         <v>29</v>
       </c>
@@ -3465,28 +3615,28 @@
       </c>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
-      <c r="H87" s="64"/>
-      <c r="I87" s="65"/>
+      <c r="H87" s="81"/>
+      <c r="I87" s="84"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="74"/>
+      <c r="A88" s="78"/>
       <c r="B88" s="61"/>
-      <c r="C88" s="76"/>
+      <c r="C88" s="90"/>
       <c r="D88" s="11" t="s">
         <v>139</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
-      <c r="H88" s="46"/>
-      <c r="I88" s="65"/>
+      <c r="H88" s="82"/>
+      <c r="I88" s="89"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="74"/>
+      <c r="A89" s="78"/>
       <c r="B89" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="C89" s="76" t="s">
+      <c r="C89" s="90" t="s">
         <v>137</v>
       </c>
       <c r="D89" s="9" t="s">
@@ -3498,14 +3648,20 @@
       <c r="F89" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="G89" s="10"/>
-      <c r="H89" s="53"/>
-      <c r="I89" s="55"/>
+      <c r="G89" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H89" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I89" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="74"/>
+      <c r="A90" s="78"/>
       <c r="B90" s="61"/>
-      <c r="C90" s="76"/>
+      <c r="C90" s="90"/>
       <c r="D90" s="10" t="s">
         <v>140</v>
       </c>
@@ -3514,30 +3670,30 @@
       </c>
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
-      <c r="H90" s="64"/>
-      <c r="I90" s="65"/>
+      <c r="H90" s="81"/>
+      <c r="I90" s="84"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="75"/>
+      <c r="A91" s="79"/>
       <c r="B91" s="67"/>
-      <c r="C91" s="77"/>
+      <c r="C91" s="91"/>
       <c r="D91" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E91" s="17"/>
       <c r="F91" s="16"/>
       <c r="G91" s="16"/>
-      <c r="H91" s="54"/>
-      <c r="I91" s="56"/>
+      <c r="H91" s="86"/>
+      <c r="I91" s="84"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="73" t="s">
+      <c r="A92" s="77" t="s">
         <v>130</v>
       </c>
       <c r="B92" s="60" t="s">
         <v>133</v>
       </c>
-      <c r="C92" s="78" t="s">
+      <c r="C92" s="92" t="s">
         <v>136</v>
       </c>
       <c r="D92" s="14" t="s">
@@ -3549,14 +3705,20 @@
       <c r="F92" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G92" s="14"/>
-      <c r="H92" s="45"/>
-      <c r="I92" s="47"/>
+      <c r="G92" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="H92" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I92" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="74"/>
+      <c r="A93" s="78"/>
       <c r="B93" s="61"/>
-      <c r="C93" s="76"/>
+      <c r="C93" s="90"/>
       <c r="D93" s="10" t="s">
         <v>22</v>
       </c>
@@ -3565,28 +3727,28 @@
       </c>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
-      <c r="H93" s="64"/>
-      <c r="I93" s="65"/>
+      <c r="H93" s="81"/>
+      <c r="I93" s="84"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="74"/>
+      <c r="A94" s="78"/>
       <c r="B94" s="61"/>
-      <c r="C94" s="76"/>
+      <c r="C94" s="90"/>
       <c r="D94" s="11" t="s">
         <v>139</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
-      <c r="H94" s="46"/>
-      <c r="I94" s="65"/>
+      <c r="H94" s="82"/>
+      <c r="I94" s="89"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="74"/>
+      <c r="A95" s="78"/>
       <c r="B95" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="C95" s="76" t="s">
+      <c r="C95" s="90" t="s">
         <v>135</v>
       </c>
       <c r="D95" s="9" t="s">
@@ -3598,14 +3760,20 @@
       <c r="F95" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="G95" s="10"/>
-      <c r="H95" s="53"/>
-      <c r="I95" s="55"/>
+      <c r="G95" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H95" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I95" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="74"/>
+      <c r="A96" s="78"/>
       <c r="B96" s="61"/>
-      <c r="C96" s="76"/>
+      <c r="C96" s="90"/>
       <c r="D96" s="10" t="s">
         <v>140</v>
       </c>
@@ -3614,30 +3782,30 @@
       </c>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
-      <c r="H96" s="64"/>
-      <c r="I96" s="65"/>
+      <c r="H96" s="81"/>
+      <c r="I96" s="84"/>
     </row>
     <row r="97" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="75"/>
+      <c r="A97" s="79"/>
       <c r="B97" s="67"/>
-      <c r="C97" s="77"/>
+      <c r="C97" s="91"/>
       <c r="D97" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E97" s="17"/>
       <c r="F97" s="16"/>
       <c r="G97" s="16"/>
-      <c r="H97" s="54"/>
-      <c r="I97" s="56"/>
+      <c r="H97" s="86"/>
+      <c r="I97" s="84"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="73" t="s">
+      <c r="A98" s="77" t="s">
         <v>143</v>
       </c>
       <c r="B98" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="C98" s="78" t="s">
+      <c r="C98" s="92" t="s">
         <v>152</v>
       </c>
       <c r="D98" s="14" t="s">
@@ -3649,14 +3817,20 @@
       <c r="F98" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G98" s="14"/>
-      <c r="H98" s="45"/>
-      <c r="I98" s="47"/>
+      <c r="G98" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H98" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I98" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="74"/>
+      <c r="A99" s="78"/>
       <c r="B99" s="61"/>
-      <c r="C99" s="76"/>
+      <c r="C99" s="90"/>
       <c r="D99" s="10" t="s">
         <v>29</v>
       </c>
@@ -3665,28 +3839,28 @@
       </c>
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
-      <c r="H99" s="64"/>
-      <c r="I99" s="65"/>
+      <c r="H99" s="81"/>
+      <c r="I99" s="84"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="74"/>
+      <c r="A100" s="78"/>
       <c r="B100" s="61"/>
-      <c r="C100" s="76"/>
+      <c r="C100" s="90"/>
       <c r="D100" s="11" t="s">
         <v>150</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="11"/>
       <c r="G100" s="11"/>
-      <c r="H100" s="46"/>
-      <c r="I100" s="65"/>
+      <c r="H100" s="82"/>
+      <c r="I100" s="89"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="74"/>
+      <c r="A101" s="78"/>
       <c r="B101" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="C101" s="76" t="s">
+      <c r="C101" s="90" t="s">
         <v>153</v>
       </c>
       <c r="D101" s="9" t="s">
@@ -3698,14 +3872,20 @@
       <c r="F101" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="G101" s="10"/>
-      <c r="H101" s="53"/>
-      <c r="I101" s="55"/>
+      <c r="G101" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="H101" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I101" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="74"/>
+      <c r="A102" s="78"/>
       <c r="B102" s="61"/>
-      <c r="C102" s="76"/>
+      <c r="C102" s="90"/>
       <c r="D102" s="10" t="s">
         <v>151</v>
       </c>
@@ -3714,30 +3894,30 @@
       </c>
       <c r="F102" s="10"/>
       <c r="G102" s="10"/>
-      <c r="H102" s="64"/>
-      <c r="I102" s="65"/>
+      <c r="H102" s="81"/>
+      <c r="I102" s="84"/>
     </row>
     <row r="103" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="75"/>
+      <c r="A103" s="79"/>
       <c r="B103" s="67"/>
-      <c r="C103" s="77"/>
+      <c r="C103" s="91"/>
       <c r="D103" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E103" s="17"/>
       <c r="F103" s="16"/>
       <c r="G103" s="16"/>
-      <c r="H103" s="54"/>
-      <c r="I103" s="56"/>
+      <c r="H103" s="86"/>
+      <c r="I103" s="84"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="73" t="s">
+      <c r="A104" s="77" t="s">
         <v>144</v>
       </c>
       <c r="B104" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="C104" s="78" t="s">
+      <c r="C104" s="92" t="s">
         <v>154</v>
       </c>
       <c r="D104" s="14" t="s">
@@ -3749,14 +3929,20 @@
       <c r="F104" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="G104" s="14"/>
-      <c r="H104" s="45"/>
-      <c r="I104" s="47"/>
+      <c r="G104" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H104" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I104" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="74"/>
+      <c r="A105" s="78"/>
       <c r="B105" s="61"/>
-      <c r="C105" s="76"/>
+      <c r="C105" s="90"/>
       <c r="D105" s="10" t="s">
         <v>22</v>
       </c>
@@ -3765,28 +3951,28 @@
       </c>
       <c r="F105" s="10"/>
       <c r="G105" s="10"/>
-      <c r="H105" s="64"/>
-      <c r="I105" s="65"/>
+      <c r="H105" s="81"/>
+      <c r="I105" s="84"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="74"/>
+      <c r="A106" s="78"/>
       <c r="B106" s="61"/>
-      <c r="C106" s="76"/>
+      <c r="C106" s="90"/>
       <c r="D106" s="11" t="s">
         <v>150</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="11"/>
       <c r="G106" s="11"/>
-      <c r="H106" s="46"/>
-      <c r="I106" s="65"/>
+      <c r="H106" s="82"/>
+      <c r="I106" s="89"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="74"/>
+      <c r="A107" s="78"/>
       <c r="B107" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="C107" s="76" t="s">
+      <c r="C107" s="90" t="s">
         <v>155</v>
       </c>
       <c r="D107" s="9" t="s">
@@ -3798,14 +3984,20 @@
       <c r="F107" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="G107" s="10"/>
-      <c r="H107" s="53"/>
-      <c r="I107" s="55"/>
+      <c r="G107" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="H107" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I107" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="74"/>
+      <c r="A108" s="78"/>
       <c r="B108" s="61"/>
-      <c r="C108" s="76"/>
+      <c r="C108" s="90"/>
       <c r="D108" s="10" t="s">
         <v>149</v>
       </c>
@@ -3814,30 +4006,30 @@
       </c>
       <c r="F108" s="10"/>
       <c r="G108" s="10"/>
-      <c r="H108" s="64"/>
-      <c r="I108" s="65"/>
+      <c r="H108" s="81"/>
+      <c r="I108" s="84"/>
     </row>
     <row r="109" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="75"/>
+      <c r="A109" s="79"/>
       <c r="B109" s="67"/>
-      <c r="C109" s="77"/>
+      <c r="C109" s="91"/>
       <c r="D109" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E109" s="17"/>
       <c r="F109" s="16"/>
       <c r="G109" s="16"/>
-      <c r="H109" s="54"/>
-      <c r="I109" s="56"/>
+      <c r="H109" s="86"/>
+      <c r="I109" s="84"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="73" t="s">
+      <c r="A110" s="77" t="s">
         <v>162</v>
       </c>
       <c r="B110" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="C110" s="78" t="s">
+      <c r="C110" s="92" t="s">
         <v>174</v>
       </c>
       <c r="D110" s="14" t="s">
@@ -3849,14 +4041,20 @@
       <c r="F110" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="G110" s="14"/>
-      <c r="H110" s="45"/>
-      <c r="I110" s="47"/>
+      <c r="G110" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="H110" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I110" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="74"/>
+      <c r="A111" s="78"/>
       <c r="B111" s="61"/>
-      <c r="C111" s="76"/>
+      <c r="C111" s="90"/>
       <c r="D111" s="10" t="s">
         <v>29</v>
       </c>
@@ -3865,28 +4063,28 @@
       </c>
       <c r="F111" s="10"/>
       <c r="G111" s="10"/>
-      <c r="H111" s="64"/>
-      <c r="I111" s="65"/>
+      <c r="H111" s="81"/>
+      <c r="I111" s="84"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="74"/>
+      <c r="A112" s="78"/>
       <c r="B112" s="61"/>
-      <c r="C112" s="76"/>
+      <c r="C112" s="90"/>
       <c r="D112" s="11" t="s">
         <v>169</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="11"/>
       <c r="G112" s="11"/>
-      <c r="H112" s="46"/>
-      <c r="I112" s="65"/>
+      <c r="H112" s="82"/>
+      <c r="I112" s="89"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="74"/>
+      <c r="A113" s="78"/>
       <c r="B113" s="61" t="s">
         <v>165</v>
       </c>
-      <c r="C113" s="76" t="s">
+      <c r="C113" s="90" t="s">
         <v>173</v>
       </c>
       <c r="D113" s="9" t="s">
@@ -3898,14 +4096,20 @@
       <c r="F113" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G113" s="10"/>
-      <c r="H113" s="53"/>
-      <c r="I113" s="55"/>
+      <c r="G113" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H113" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I113" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="74"/>
+      <c r="A114" s="78"/>
       <c r="B114" s="61"/>
-      <c r="C114" s="76"/>
+      <c r="C114" s="90"/>
       <c r="D114" s="10" t="s">
         <v>170</v>
       </c>
@@ -3914,30 +4118,30 @@
       </c>
       <c r="F114" s="10"/>
       <c r="G114" s="10"/>
-      <c r="H114" s="64"/>
-      <c r="I114" s="65"/>
+      <c r="H114" s="81"/>
+      <c r="I114" s="84"/>
     </row>
     <row r="115" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="75"/>
+      <c r="A115" s="79"/>
       <c r="B115" s="67"/>
-      <c r="C115" s="77"/>
+      <c r="C115" s="91"/>
       <c r="D115" s="16" t="s">
         <v>45</v>
       </c>
       <c r="E115" s="17"/>
       <c r="F115" s="16"/>
       <c r="G115" s="16"/>
-      <c r="H115" s="54"/>
-      <c r="I115" s="56"/>
+      <c r="H115" s="86"/>
+      <c r="I115" s="84"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="73" t="s">
+      <c r="A116" s="77" t="s">
         <v>163</v>
       </c>
       <c r="B116" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="C116" s="78" t="s">
+      <c r="C116" s="92" t="s">
         <v>172</v>
       </c>
       <c r="D116" s="14" t="s">
@@ -3949,14 +4153,20 @@
       <c r="F116" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="G116" s="14"/>
-      <c r="H116" s="45"/>
-      <c r="I116" s="47"/>
+      <c r="G116" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="H116" s="80" t="s">
+        <v>305</v>
+      </c>
+      <c r="I116" s="83" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="74"/>
+      <c r="A117" s="78"/>
       <c r="B117" s="61"/>
-      <c r="C117" s="76"/>
+      <c r="C117" s="90"/>
       <c r="D117" s="10" t="s">
         <v>22</v>
       </c>
@@ -3965,28 +4175,28 @@
       </c>
       <c r="F117" s="10"/>
       <c r="G117" s="10"/>
-      <c r="H117" s="64"/>
-      <c r="I117" s="65"/>
+      <c r="H117" s="81"/>
+      <c r="I117" s="84"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="74"/>
+      <c r="A118" s="78"/>
       <c r="B118" s="61"/>
-      <c r="C118" s="76"/>
+      <c r="C118" s="90"/>
       <c r="D118" s="11" t="s">
         <v>169</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="11"/>
       <c r="G118" s="11"/>
-      <c r="H118" s="46"/>
-      <c r="I118" s="65"/>
+      <c r="H118" s="82"/>
+      <c r="I118" s="89"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="74"/>
+      <c r="A119" s="78"/>
       <c r="B119" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="C119" s="76" t="s">
+      <c r="C119" s="90" t="s">
         <v>171</v>
       </c>
       <c r="D119" s="9" t="s">
@@ -3998,14 +4208,20 @@
       <c r="F119" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G119" s="10"/>
-      <c r="H119" s="53"/>
-      <c r="I119" s="55"/>
+      <c r="G119" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="H119" s="85" t="s">
+        <v>305</v>
+      </c>
+      <c r="I119" s="84" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="74"/>
+      <c r="A120" s="78"/>
       <c r="B120" s="61"/>
-      <c r="C120" s="76"/>
+      <c r="C120" s="90"/>
       <c r="D120" s="10" t="s">
         <v>168</v>
       </c>
@@ -4014,21 +4230,21 @@
       </c>
       <c r="F120" s="10"/>
       <c r="G120" s="10"/>
-      <c r="H120" s="64"/>
-      <c r="I120" s="65"/>
+      <c r="H120" s="81"/>
+      <c r="I120" s="84"/>
     </row>
     <row r="121" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="75"/>
+      <c r="A121" s="79"/>
       <c r="B121" s="67"/>
-      <c r="C121" s="77"/>
+      <c r="C121" s="91"/>
       <c r="D121" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E121" s="17"/>
       <c r="F121" s="16"/>
       <c r="G121" s="16"/>
-      <c r="H121" s="54"/>
-      <c r="I121" s="56"/>
+      <c r="H121" s="86"/>
+      <c r="I121" s="84"/>
     </row>
     <row r="122" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="38" t="s">

</xml_diff>